<commit_message>
changes as of 17/july/2017
</commit_message>
<xml_diff>
--- a/RPC_XML_Data.xlsx
+++ b/RPC_XML_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>FilterData</t>
   </si>
@@ -108,13 +108,6 @@
     <t>show running-config | include console</t>
   </si>
   <si>
-    <t>&lt;sys:syslog xmlns:sys="urn:ietf:params:xml:ns:yang:ietf-syslog"&gt;
-         &lt;sys:remote-logging-action&gt;
-                &lt;sys:remote-logging-destination/&gt;
-         &lt;/sys:remote-logging-action&gt;
-&lt;/sys:syslog&gt;</t>
-  </si>
-  <si>
     <t>logging host "1.2.3.4" ipv4 12345 warning</t>
   </si>
   <si>
@@ -160,26 +153,54 @@
  &lt;/nc:config&gt;</t>
   </si>
   <si>
+    <t>&lt;sys:syslog xmlns:sys="urn:ietf:params:xml:ns:yang:ietf-syslog"&gt;
+         &lt;sys:remote-logging-action&gt;
+                  &lt;sys:remote-logging-destination/&gt;
+        &lt;/sys:remote-logging-action&gt;
+&lt;/sys:syslog&gt;</t>
+  </si>
+  <si>
     <t>&lt;nc:config xmlns:nc="urn:ietf:params:xml:ns:netconf:base:1.0"&gt;
-         &lt;if:interfaces xmlns:if="urn:ietf:params:xml:ns:yang:ietf-interfaces"&gt;
-                &lt;if:interface nc:operation="merge"&gt;
-                       &lt;if:name&gt;0/1&lt;/if:name&gt;
-                        &lt;ip:ipv4 xmlns:ip="urn:ietf:params:xml:ns:yang:ietf-ip"&gt;
+        &lt;if:interfaces xmlns:if="urn:ietf:params:xml:ns:yang:ietf-interfaces"&gt;
+               &lt;if:interface nc:operation="merge"&gt;
+                      &lt;if:name&gt;0/1&lt;/if:name&gt;
+                      &lt;ip:ipv4 xmlns:ip="urn:ietf:params:xml:ns:yang:ietf-ip"&gt;
                                &lt;ip:enabled&gt;true&lt;/ip:enabled&gt;
-                         &lt;/ip:ipv4&gt;
-                   &lt;/if:interface&gt;
+                      &lt;/ip:ipv4&gt;
+               &lt;/if:interface&gt;
           &lt;/if:interfaces&gt;
           &lt;syslog xmlns="urn:ietf:params:xml:ns:yang:ietf-syslog"&gt;
-                  &lt;remote-logging-action nc:operation="merge"&gt;
-                           &lt;remote-logging-destination&gt;
-                                    &lt;destination&gt;1.2.3.4&lt;/destination&gt;
-                                     &lt;destination-port&gt;123&lt;/destination-port&gt;
-                                      &lt;severity&gt;notice&lt;/severity&gt;
-                                      &lt;source-interface xmlns:if="urn:ietf:params:xml:ns:yang:ietf-interfaces"&gt;0/1&lt;/source-interface&gt;
-                             &lt;/remote-logging-destination&gt;
-                     &lt;/remote-logging-action&gt;
-            &lt;/syslog&gt;
+                 &lt;remote-logging-action nc:operation="%s"&gt;
+                         &lt;remote-logging-destination&gt;
+                                            &lt;destination&gt;1.2.3.4&lt;/destination&gt;
+                                            &lt;destination-port&gt;123&lt;/destination-port&gt;
+                                            &lt;severity&gt;notice&lt;/severity&gt;
+                                            &lt;source-interface xmlns:if="urn:ietf:params:xml:ns:yang:ietf-interfaces"&gt;0/1&lt;/source-interface&gt;
+                        &lt;/remote-logging-destination&gt;
+                 &lt;/remote-logging-action&gt;
+           &lt;/syslog&gt;
 &lt;/nc:config&gt;</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>link-up-down-trap-enable</t>
+  </si>
+  <si>
+    <t>buffered-logging-action</t>
+  </si>
+  <si>
+    <t>remote-logging-destination</t>
+  </si>
+  <si>
+    <t>console-logging-action</t>
   </si>
 </sst>
 </file>
@@ -558,129 +579,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91" customWidth="1"/>
-    <col min="2" max="2" width="88.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91" customWidth="1"/>
+    <col min="3" max="3" width="88.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -690,74 +670,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91" customWidth="1"/>
-    <col min="2" max="2" width="88.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91" customWidth="1"/>
+    <col min="3" max="3" width="88.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="315" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>